<commit_message>
itergrated both parsers of excel files into a single one. Corrected minor frondend errors
</commit_message>
<xml_diff>
--- a/src/main/resources/data/samples/sample.xlsx
+++ b/src/main/resources/data/samples/sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">csvFile</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t xml:space="preserve">methodology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mapFunction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mapCDE</t>
   </si>
 </sst>
 </file>
@@ -103,17 +109,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00CCFF"/>
-        <bgColor rgb="FF33CCCC"/>
+        <fgColor rgb="FF33FF99"/>
+        <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="double"/>
+      <right style="double"/>
+      <top style="double"/>
+      <bottom style="double"/>
       <diagonal/>
     </border>
   </borders>
@@ -142,12 +155,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -160,6 +177,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33FF99"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -168,18 +245,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.1938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -212,6 +291,12 @@
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>